<commit_message>
[ NEW ] Test Added
</commit_message>
<xml_diff>
--- a/public/excel/user.xlsx
+++ b/public/excel/user.xlsx
@@ -24,12 +24,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Bala</t>
-  </si>
-  <si>
-    <t>Chandran</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -69,12 +63,6 @@
     <t>Group_Id</t>
   </si>
   <si>
-    <t>rbalabca@gmail.com</t>
-  </si>
-  <si>
-    <t>rbalachandranmca@gmail.com</t>
-  </si>
-  <si>
     <t>Sample Address 1</t>
   </si>
   <si>
@@ -93,16 +81,28 @@
     <t>a234567</t>
   </si>
   <si>
-    <t>sam12@gmail.com</t>
-  </si>
-  <si>
-    <t>sam23@gmail.com</t>
-  </si>
-  <si>
-    <t>Bala2</t>
-  </si>
-  <si>
-    <t>Chandran3</t>
+    <t>ben@gmail.com</t>
+  </si>
+  <si>
+    <t>gwen@gmail.com</t>
+  </si>
+  <si>
+    <t>jarvis@gmail.com</t>
+  </si>
+  <si>
+    <t>tony@gmail.com</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Jarvis</t>
+  </si>
+  <si>
+    <t>Gwen</t>
+  </si>
+  <si>
+    <t>Tony</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -466,78 +466,78 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4">
         <v>33229</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E2">
         <v>9998758974</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H2">
         <v>9887439874</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="K2" s="6">
         <v>1</v>
@@ -554,34 +554,34 @@
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="C3" s="4">
         <v>33960</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>8889807434</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H3">
         <v>9789743987</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K3">
         <v>1</v>

</xml_diff>